<commit_message>
Commiting new updates in switching file
</commit_message>
<xml_diff>
--- a/Course_JAVA/Switching.xlsx
+++ b/Course_JAVA/Switching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBD5\Desktop\Kiran\2025_Preparation\Java_Programms_2024\Course_JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4788E063-7C39-4C2F-990A-784C8AA46BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464A46EF-EA5B-4BE1-ADA3-6DB7FE65C5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AC86AE55-8C37-4AF0-8211-798EC76903A2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>SUBJECTS</t>
   </si>
@@ -211,13 +211,79 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=SniLNfFejiU</t>
+  </si>
+  <si>
+    <t>Stale Element Exception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Element not found
+&gt; This error occurs when the element is not present in the HTML code. This can be caused by wrong selectors, missing waits, or navigation problems. 
+2. Element not visible
+&gt; This error occurs when the element is present in the HTML code but is hidden. This can happen if the element is covered by another element, disabled, or outside the viewport. </t>
+  </si>
+  <si>
+    <t>Framework Tricky Questions Rahul Shetty</t>
+  </si>
+  <si>
+    <t>Udemy Selenium Course</t>
+  </si>
+  <si>
+    <t>Capgemini Interview Questions - Bengaluru location</t>
+  </si>
+  <si>
+    <t>1. I want to ensure a new element got added to drop-down how to do that.</t>
+  </si>
+  <si>
+    <t>2. Have you worked on Jenkins Implementation in frameworks like Selenium, restAssured</t>
+  </si>
+  <si>
+    <t>3. Write regular expression for email input</t>
+  </si>
+  <si>
+    <t>4. Write code for web-table automation, I want to fetch 2nd row and 3rd coloumn cell value.</t>
+  </si>
+  <si>
+    <t>5. When you will get stale element Exception</t>
+  </si>
+  <si>
+    <t>Capgemini Interview Questions - Chennai location</t>
+  </si>
+  <si>
+    <t>1. Difference between Element Not Found and Element not visible Exception</t>
+  </si>
+  <si>
+    <t>2. Difference between oAuth1 and oAuth2</t>
+  </si>
+  <si>
+    <t>3. why 402 comes</t>
+  </si>
+  <si>
+    <t>4. What is parameterization in selenium and how it is achived</t>
+  </si>
+  <si>
+    <t>5. Explain how you implemented OOPs concepts in your framework</t>
+  </si>
+  <si>
+    <t>6. Explain Framework Structure</t>
+  </si>
+  <si>
+    <t>7. How to implement multithreading in Framework</t>
+  </si>
+  <si>
+    <t>8. What is the limit of priority in TestNG and what will happen if we giv -ve priority to test case.</t>
+  </si>
+  <si>
+    <t>9. Fibonacci series and patteren program for the below patteren                                                                                            1                                                                            12                                                                  123                                                                1234                                                       12345</t>
+  </si>
+  <si>
+    <t>10. Selenium 4 features</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,8 +313,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -314,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -325,9 +405,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -355,10 +432,28 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -676,16 +771,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45323040-EFC5-4F86-BB27-0E93C4A8D5B8}">
-  <dimension ref="C5:L17"/>
+  <dimension ref="C1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="18.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="71.81640625" style="13" customWidth="1"/>
     <col min="4" max="4" width="27.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="1" bestFit="1" customWidth="1"/>
@@ -698,269 +793,371 @@
     <col min="13" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
+    <row r="1" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C1" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C17" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="16"/>
+      <c r="D21" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C6" s="3" t="s">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="H6" s="6" t="s">
+      <c r="D22" s="2"/>
+      <c r="H22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8" t="s">
+      <c r="J22" s="6"/>
+      <c r="K22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L22" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="4">
+    <row r="23" spans="3:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="18">
         <v>45597</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E23" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="F23" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="3:12" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="C8" s="4">
+    <row r="24" spans="3:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C24" s="18">
         <v>45658</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="1" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I24" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L24" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="3:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="4">
+    <row r="25" spans="3:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="18">
         <v>45689</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="1" t="s">
+      <c r="E25" s="14"/>
+      <c r="F25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G25" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I25" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L25" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="3:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="4">
+    <row r="26" spans="3:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="18">
         <v>45717</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="1" t="s">
+      <c r="E26" s="14"/>
+      <c r="F26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G26" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L26" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="4">
+    <row r="27" spans="3:12" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="18">
         <v>45748</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="1" t="s">
+      <c r="E27" s="14"/>
+      <c r="F27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G27" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I27" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K27" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L27" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="H12" s="9" t="s">
+    <row r="28" spans="3:12" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="F28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L28" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="3:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="H13" s="9" t="s">
+    <row r="29" spans="3:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="H29" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L29" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="H14" s="9" t="s">
+    <row r="30" spans="3:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="H30" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I30" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K30" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L30" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="3:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="H15" s="9" t="s">
+    <row r="31" spans="3:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="H31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I31" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K31" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L31" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="3:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="H16" s="11" t="s">
+    <row r="32" spans="3:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="H32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I32" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K32" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L32" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="11:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="K17" s="12" t="s">
+    <row r="33" spans="11:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L33" s="12" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E23:E27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1" xr:uid="{19B8B9A6-0D14-4DF7-83D4-6EAC417EFFBF}"/>
-    <hyperlink ref="I8" r:id="rId2" location="google_vignette" xr:uid="{8F2FC74F-48B1-4ABF-B361-65859470B6EB}"/>
-    <hyperlink ref="L7" r:id="rId3" xr:uid="{483B4E20-5184-47A5-AF69-7B44A995F6AA}"/>
-    <hyperlink ref="L8" r:id="rId4" xr:uid="{2A23487F-1CA6-43CE-9665-70A0F48DDB22}"/>
-    <hyperlink ref="L9" r:id="rId5" xr:uid="{FCE87965-9101-48B4-9186-55023E56E702}"/>
-    <hyperlink ref="L10" r:id="rId6" xr:uid="{1760EFF8-3E6F-45E5-90A5-F4842E46222D}"/>
-    <hyperlink ref="L12" r:id="rId7" xr:uid="{AC2D21D1-7427-4C76-B3C5-F815D66A541A}"/>
-    <hyperlink ref="I12" r:id="rId8" xr:uid="{FA68B5D9-9717-45F6-91E7-1A831AC6DDB7}"/>
-    <hyperlink ref="I13" r:id="rId9" xr:uid="{3375D102-B005-4925-A521-0B150653326D}"/>
-    <hyperlink ref="I14" r:id="rId10" xr:uid="{68DED11B-E156-4B73-899E-0DF969096F61}"/>
-    <hyperlink ref="L13" r:id="rId11" xr:uid="{3E9BD190-E87C-4307-B3A8-F1229FCBEE64}"/>
-    <hyperlink ref="L14" r:id="rId12" xr:uid="{05D44AF7-B62F-4EA5-9144-2069BDB53D5C}"/>
-    <hyperlink ref="L15" r:id="rId13" xr:uid="{B8C17712-FAF2-4396-B24B-3265EB00B649}"/>
-    <hyperlink ref="L16" r:id="rId14" xr:uid="{763BD6A2-D97B-4367-B9E8-A9904AD0A905}"/>
-    <hyperlink ref="L17" r:id="rId15" xr:uid="{6E207B70-01EB-46C8-86D5-38C4641ACDAD}"/>
-    <hyperlink ref="I15" r:id="rId16" xr:uid="{7D74F3BB-82EC-431D-9DA0-B70917D299D9}"/>
-    <hyperlink ref="I16" r:id="rId17" xr:uid="{1471BC00-7D49-4777-9171-DFBDA2992B82}"/>
-    <hyperlink ref="I9" r:id="rId18" xr:uid="{27E4409B-91E1-4266-84CF-09E5EF42ED00}"/>
-    <hyperlink ref="L11" r:id="rId19" xr:uid="{B64768DC-3EF7-49B4-BEEA-6087DEB1A1C8}"/>
-    <hyperlink ref="I10" r:id="rId20" xr:uid="{F1B52C8A-8CA7-4E55-AE9C-B19A0A17AE62}"/>
-    <hyperlink ref="I11" r:id="rId21" xr:uid="{0243746E-78E6-4C63-8A6A-935AFF113CA2}"/>
+    <hyperlink ref="I23" r:id="rId1" xr:uid="{19B8B9A6-0D14-4DF7-83D4-6EAC417EFFBF}"/>
+    <hyperlink ref="I24" r:id="rId2" location="google_vignette" xr:uid="{8F2FC74F-48B1-4ABF-B361-65859470B6EB}"/>
+    <hyperlink ref="L23" r:id="rId3" xr:uid="{483B4E20-5184-47A5-AF69-7B44A995F6AA}"/>
+    <hyperlink ref="L24" r:id="rId4" xr:uid="{2A23487F-1CA6-43CE-9665-70A0F48DDB22}"/>
+    <hyperlink ref="L25" r:id="rId5" xr:uid="{FCE87965-9101-48B4-9186-55023E56E702}"/>
+    <hyperlink ref="L26" r:id="rId6" xr:uid="{1760EFF8-3E6F-45E5-90A5-F4842E46222D}"/>
+    <hyperlink ref="L28" r:id="rId7" xr:uid="{AC2D21D1-7427-4C76-B3C5-F815D66A541A}"/>
+    <hyperlink ref="I28" r:id="rId8" xr:uid="{FA68B5D9-9717-45F6-91E7-1A831AC6DDB7}"/>
+    <hyperlink ref="I29" r:id="rId9" xr:uid="{3375D102-B005-4925-A521-0B150653326D}"/>
+    <hyperlink ref="I30" r:id="rId10" xr:uid="{68DED11B-E156-4B73-899E-0DF969096F61}"/>
+    <hyperlink ref="L29" r:id="rId11" xr:uid="{3E9BD190-E87C-4307-B3A8-F1229FCBEE64}"/>
+    <hyperlink ref="L30" r:id="rId12" xr:uid="{05D44AF7-B62F-4EA5-9144-2069BDB53D5C}"/>
+    <hyperlink ref="L31" r:id="rId13" xr:uid="{B8C17712-FAF2-4396-B24B-3265EB00B649}"/>
+    <hyperlink ref="L32" r:id="rId14" xr:uid="{763BD6A2-D97B-4367-B9E8-A9904AD0A905}"/>
+    <hyperlink ref="L33" r:id="rId15" xr:uid="{6E207B70-01EB-46C8-86D5-38C4641ACDAD}"/>
+    <hyperlink ref="I31" r:id="rId16" xr:uid="{7D74F3BB-82EC-431D-9DA0-B70917D299D9}"/>
+    <hyperlink ref="I32" r:id="rId17" xr:uid="{1471BC00-7D49-4777-9171-DFBDA2992B82}"/>
+    <hyperlink ref="I25" r:id="rId18" xr:uid="{27E4409B-91E1-4266-84CF-09E5EF42ED00}"/>
+    <hyperlink ref="L27" r:id="rId19" xr:uid="{B64768DC-3EF7-49B4-BEEA-6087DEB1A1C8}"/>
+    <hyperlink ref="I26" r:id="rId20" xr:uid="{F1B52C8A-8CA7-4E55-AE9C-B19A0A17AE62}"/>
+    <hyperlink ref="I27" r:id="rId21" xr:uid="{0243746E-78E6-4C63-8A6A-935AFF113CA2}"/>
+    <hyperlink ref="G24" r:id="rId22" xr:uid="{86E595F1-5422-4FA4-B0D6-B29C929C708D}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{FD34B623-D54B-4D83-B1F0-D8B1914457AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>